<commit_message>
Fix Overall Response BC
</commit_message>
<xml_diff>
--- a/curation/draft/BC_Package_R8_BC_updates.xlsx
+++ b/curation/draft/BC_Package_R8_BC_updates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Linda\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\curation\draft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{862EBA2E-F97D-4CEF-AB78-4B7DA0F698FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC4852E-15EB-446F-A7BF-05E5C7923B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="390" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BC_Onco_Corrections" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1775" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1775" uniqueCount="209">
   <si>
     <t>package_date</t>
   </si>
@@ -607,9 +607,6 @@
   </si>
   <si>
     <t>The determination of the amount of very low-density lipoprotein cholesterol present in a sample.</t>
-  </si>
-  <si>
-    <t>Oncology Standards; Disease Response; Disease Response Criteria; Disease Response and Clinical Classification; RS; RECIST 1.1; iRECIST; LUGANO; RANO; iRANO; POINTE-DI-LEGNO; RAJKUMARMM</t>
   </si>
   <si>
     <t>Oncology Standards; Disease Response; Disease Response Criteria; Disease Response and Clinical Classification; RS; RECIST 1.0; iRECIST</t>
@@ -661,7 +658,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="9.5"/>
       <color rgb="FF000000"/>
@@ -954,32 +951,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.6875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6875" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="50.3125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.6875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.6875" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="55.6875" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.6875" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.6875" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.6875" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.6875" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.6875" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.4375" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.6875" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="55.6875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="50.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="55.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="55.7109375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="14.1" customHeight="1">
+    <row r="1" spans="1:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1032,10 +1029,10 @@
         <v>16</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="57.95" customHeight="1">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>122</v>
       </c>
@@ -1052,7 +1049,7 @@
         <v>23</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>24</v>
@@ -1085,7 +1082,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="57.95" customHeight="1">
+    <row r="3" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>122</v>
       </c>
@@ -1102,7 +1099,7 @@
         <v>23</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>24</v>
@@ -1132,7 +1129,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="57.95" customHeight="1">
+    <row r="4" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>122</v>
       </c>
@@ -1149,7 +1146,7 @@
         <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>24</v>
@@ -1179,7 +1176,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="57.95" customHeight="1">
+    <row r="5" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>122</v>
       </c>
@@ -1196,7 +1193,7 @@
         <v>23</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>24</v>
@@ -1226,7 +1223,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="57.95" customHeight="1">
+    <row r="6" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>122</v>
       </c>
@@ -1243,7 +1240,7 @@
         <v>23</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>24</v>
@@ -1271,7 +1268,7 @@
       </c>
       <c r="Q6" s="3"/>
     </row>
-    <row r="7" spans="1:18" ht="57.95" customHeight="1">
+    <row r="7" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>122</v>
       </c>
@@ -1321,7 +1318,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="57.95" customHeight="1">
+    <row r="8" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>122</v>
       </c>
@@ -1368,7 +1365,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="57.95" customHeight="1">
+    <row r="9" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
@@ -1397,7 +1394,7 @@
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
     </row>
-    <row r="10" spans="1:18" s="11" customFormat="1" ht="57.95" customHeight="1">
+    <row r="10" spans="1:18" s="11" customFormat="1" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>122</v>
       </c>
@@ -1444,7 +1441,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="57.95" customHeight="1">
+    <row r="11" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>122</v>
       </c>
@@ -1491,7 +1488,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="57.95" customHeight="1">
+    <row r="12" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>122</v>
       </c>
@@ -1538,7 +1535,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="57.95" customHeight="1">
+    <row r="13" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>122</v>
       </c>
@@ -1585,7 +1582,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="57.95" customHeight="1">
+    <row r="14" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>122</v>
       </c>
@@ -1632,7 +1629,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="57.95" customHeight="1">
+    <row r="15" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>122</v>
       </c>
@@ -1679,7 +1676,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="57.95" customHeight="1">
+    <row r="16" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>122</v>
       </c>
@@ -1724,7 +1721,7 @@
       </c>
       <c r="Q16" s="3"/>
     </row>
-    <row r="17" spans="1:18" ht="57.95" customHeight="1">
+    <row r="17" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>122</v>
       </c>
@@ -1774,7 +1771,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="57.95" customHeight="1">
+    <row r="18" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>122</v>
       </c>
@@ -1821,7 +1818,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="57.95" customHeight="1">
+    <row r="19" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>122</v>
       </c>
@@ -1868,7 +1865,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="57.95" customHeight="1">
+    <row r="20" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>122</v>
       </c>
@@ -1913,7 +1910,7 @@
       </c>
       <c r="Q20" s="3"/>
     </row>
-    <row r="21" spans="1:18" ht="57.95" customHeight="1">
+    <row r="21" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>122</v>
       </c>
@@ -1963,7 +1960,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="57.95" customHeight="1">
+    <row r="22" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>122</v>
       </c>
@@ -2010,7 +2007,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="57.95" customHeight="1">
+    <row r="23" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>122</v>
       </c>
@@ -2057,7 +2054,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="57.95" customHeight="1">
+    <row r="24" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>122</v>
       </c>
@@ -2102,7 +2099,7 @@
       </c>
       <c r="Q24" s="3"/>
     </row>
-    <row r="25" spans="1:18" ht="57.95" customHeight="1">
+    <row r="25" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>122</v>
       </c>
@@ -2152,7 +2149,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="57.95" customHeight="1">
+    <row r="26" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>122</v>
       </c>
@@ -2199,7 +2196,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="57.95" customHeight="1">
+    <row r="27" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>122</v>
       </c>
@@ -2246,7 +2243,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="72" customHeight="1">
+    <row r="28" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>122</v>
       </c>
@@ -2293,7 +2290,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="57.95" customHeight="1">
+    <row r="29" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>122</v>
       </c>
@@ -2340,7 +2337,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="57.95" customHeight="1">
+    <row r="30" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>122</v>
       </c>
@@ -2387,7 +2384,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="57.95" customHeight="1">
+    <row r="31" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>122</v>
       </c>
@@ -2434,7 +2431,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="57.95" customHeight="1">
+    <row r="32" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>122</v>
       </c>
@@ -2481,7 +2478,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="57.95" customHeight="1">
+    <row r="33" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>122</v>
       </c>
@@ -2528,7 +2525,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="57.95" customHeight="1">
+    <row r="34" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>122</v>
       </c>
@@ -2573,7 +2570,7 @@
       </c>
       <c r="Q34" s="3"/>
     </row>
-    <row r="35" spans="1:18" ht="57.95" customHeight="1">
+    <row r="35" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>122</v>
       </c>
@@ -2623,7 +2620,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="57.95" customHeight="1">
+    <row r="36" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>122</v>
       </c>
@@ -2670,7 +2667,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="57.95" customHeight="1">
+    <row r="37" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>122</v>
       </c>
@@ -2717,7 +2714,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="72" customHeight="1">
+    <row r="38" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>122</v>
       </c>
@@ -2764,7 +2761,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="57.95" customHeight="1">
+    <row r="39" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>122</v>
       </c>
@@ -2811,7 +2808,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="40" spans="1:18" ht="57.95" customHeight="1">
+    <row r="40" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>122</v>
       </c>
@@ -2858,7 +2855,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="57.95" customHeight="1">
+    <row r="41" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>122</v>
       </c>
@@ -2905,7 +2902,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="57.95" customHeight="1">
+    <row r="42" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>122</v>
       </c>
@@ -2952,7 +2949,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="57.95" customHeight="1">
+    <row r="43" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>122</v>
       </c>
@@ -2999,7 +2996,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="57.95" customHeight="1">
+    <row r="44" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>122</v>
       </c>
@@ -3044,7 +3041,7 @@
       </c>
       <c r="Q44" s="3"/>
     </row>
-    <row r="45" spans="1:18" ht="57.95" customHeight="1">
+    <row r="45" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>122</v>
       </c>
@@ -3061,7 +3058,7 @@
         <v>68</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>86</v>
@@ -3088,13 +3085,13 @@
         <v>20</v>
       </c>
       <c r="Q45" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="R45" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="46" spans="1:18" ht="57.95" customHeight="1">
+    <row r="46" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>122</v>
       </c>
@@ -3111,7 +3108,7 @@
         <v>68</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>86</v>
@@ -3141,7 +3138,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="57.95" customHeight="1">
+    <row r="47" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>122</v>
       </c>
@@ -3158,7 +3155,7 @@
         <v>68</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>86</v>
@@ -3188,7 +3185,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="48" spans="1:18" ht="57.95" customHeight="1">
+    <row r="48" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>122</v>
       </c>
@@ -3205,7 +3202,7 @@
         <v>68</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>86</v>
@@ -3235,7 +3232,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="57.95" customHeight="1">
+    <row r="49" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>122</v>
       </c>
@@ -3252,7 +3249,7 @@
         <v>68</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>86</v>
@@ -3280,7 +3277,7 @@
       </c>
       <c r="Q49" s="3"/>
     </row>
-    <row r="50" spans="1:18" ht="57.95" customHeight="1">
+    <row r="50" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>122</v>
       </c>
@@ -3297,7 +3294,7 @@
         <v>68</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>90</v>
@@ -3324,13 +3321,13 @@
         <v>20</v>
       </c>
       <c r="Q50" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="R50" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="57.95" customHeight="1">
+    <row r="51" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>122</v>
       </c>
@@ -3347,7 +3344,7 @@
         <v>68</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>90</v>
@@ -3377,7 +3374,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="57.95" customHeight="1">
+    <row r="52" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>122</v>
       </c>
@@ -3394,7 +3391,7 @@
         <v>68</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G52" s="3" t="s">
         <v>90</v>
@@ -3424,7 +3421,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="57.95" customHeight="1">
+    <row r="53" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>122</v>
       </c>
@@ -3441,7 +3438,7 @@
         <v>68</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>90</v>
@@ -3471,7 +3468,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="57.95" customHeight="1">
+    <row r="54" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>122</v>
       </c>
@@ -3488,7 +3485,7 @@
         <v>68</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>90</v>
@@ -3516,7 +3513,7 @@
       </c>
       <c r="Q54" s="3"/>
     </row>
-    <row r="55" spans="1:18" ht="57.95" customHeight="1">
+    <row r="55" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>122</v>
       </c>
@@ -3533,7 +3530,7 @@
         <v>68</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="G55" s="3" t="s">
         <v>95</v>
@@ -3566,7 +3563,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="56" spans="1:18" ht="57.95" customHeight="1">
+    <row r="56" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>122</v>
       </c>
@@ -3583,7 +3580,7 @@
         <v>68</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>95</v>
@@ -3610,10 +3607,10 @@
         <v>20</v>
       </c>
       <c r="Q56" s="3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18" ht="57.95" customHeight="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>122</v>
       </c>
@@ -3630,7 +3627,7 @@
         <v>68</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>95</v>
@@ -3660,7 +3657,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="58" spans="1:18" ht="57.95" customHeight="1">
+    <row r="58" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>122</v>
       </c>
@@ -3677,7 +3674,7 @@
         <v>68</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>95</v>
@@ -3707,7 +3704,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="59" spans="1:18" ht="57.95" customHeight="1">
+    <row r="59" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>122</v>
       </c>
@@ -3724,7 +3721,7 @@
         <v>68</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G59" s="3" t="s">
         <v>95</v>
@@ -3754,7 +3751,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="60" spans="1:18" ht="57.95" customHeight="1">
+    <row r="60" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>122</v>
       </c>
@@ -3771,7 +3768,7 @@
         <v>68</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G60" s="3" t="s">
         <v>95</v>
@@ -3799,7 +3796,7 @@
       </c>
       <c r="Q60" s="3"/>
     </row>
-    <row r="61" spans="1:18" ht="57.95" customHeight="1">
+    <row r="61" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>122</v>
       </c>
@@ -3849,7 +3846,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="62" spans="1:18" ht="57.95" customHeight="1">
+    <row r="62" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>122</v>
       </c>
@@ -3896,7 +3893,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="63" spans="1:18" ht="57.95" customHeight="1">
+    <row r="63" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>122</v>
       </c>
@@ -3943,7 +3940,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="64" spans="1:18" ht="72" customHeight="1">
+    <row r="64" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>122</v>
       </c>
@@ -3990,7 +3987,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="65" spans="1:18" ht="57.95" customHeight="1">
+    <row r="65" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>122</v>
       </c>
@@ -4037,7 +4034,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="66" spans="1:18" ht="57.95" customHeight="1">
+    <row r="66" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>122</v>
       </c>
@@ -4084,7 +4081,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="67" spans="1:18" ht="57.95" customHeight="1">
+    <row r="67" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>122</v>
       </c>
@@ -4131,7 +4128,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="68" spans="1:18" ht="57.95" customHeight="1">
+    <row r="68" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>122</v>
       </c>
@@ -4178,7 +4175,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="69" spans="1:18" ht="57.95" customHeight="1">
+    <row r="69" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>122</v>
       </c>
@@ -4225,7 +4222,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="70" spans="1:18" ht="57.95" customHeight="1">
+    <row r="70" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>122</v>
       </c>
@@ -4270,7 +4267,7 @@
       </c>
       <c r="Q70" s="3"/>
     </row>
-    <row r="71" spans="1:18" ht="72" customHeight="1">
+    <row r="71" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>122</v>
       </c>
@@ -4320,7 +4317,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="72" spans="1:18" ht="72" customHeight="1">
+    <row r="72" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>122</v>
       </c>
@@ -4367,7 +4364,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="73" spans="1:18" s="11" customFormat="1" ht="72" customHeight="1">
+    <row r="73" spans="1:18" s="11" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="9" t="s">
         <v>122</v>
       </c>
@@ -4414,7 +4411,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="74" spans="1:18" ht="72" customHeight="1">
+    <row r="74" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>122</v>
       </c>
@@ -4461,7 +4458,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="75" spans="1:18" ht="72" customHeight="1">
+    <row r="75" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>122</v>
       </c>
@@ -4508,7 +4505,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="76" spans="1:18" ht="72" customHeight="1">
+    <row r="76" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>122</v>
       </c>
@@ -4555,7 +4552,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="77" spans="1:18" ht="72" customHeight="1">
+    <row r="77" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>122</v>
       </c>
@@ -4602,7 +4599,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="78" spans="1:18" ht="72" customHeight="1">
+    <row r="78" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>122</v>
       </c>
@@ -4649,7 +4646,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="79" spans="1:18" ht="72" customHeight="1">
+    <row r="79" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>122</v>
       </c>
@@ -4694,7 +4691,7 @@
       </c>
       <c r="Q79" s="3"/>
     </row>
-    <row r="80" spans="1:18" ht="72" customHeight="1">
+    <row r="80" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>122</v>
       </c>
@@ -4744,7 +4741,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="81" spans="1:18" ht="72" customHeight="1">
+    <row r="81" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>122</v>
       </c>
@@ -4791,7 +4788,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="82" spans="1:18" ht="72" customHeight="1">
+    <row r="82" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>122</v>
       </c>
@@ -4838,7 +4835,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="83" spans="1:18" ht="72" customHeight="1">
+    <row r="83" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>122</v>
       </c>
@@ -4885,7 +4882,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="84" spans="1:18" ht="72" customHeight="1">
+    <row r="84" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>122</v>
       </c>
@@ -4932,7 +4929,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="85" spans="1:18" ht="72" customHeight="1">
+    <row r="85" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>122</v>
       </c>
@@ -4979,7 +4976,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="86" spans="1:18" ht="72" customHeight="1">
+    <row r="86" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>122</v>
       </c>
@@ -5026,7 +5023,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="87" spans="1:18" ht="72" customHeight="1">
+    <row r="87" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>122</v>
       </c>
@@ -5073,7 +5070,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="88" spans="1:18" ht="72" customHeight="1">
+    <row r="88" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>122</v>
       </c>
@@ -5120,7 +5117,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="89" spans="1:18" ht="72" customHeight="1">
+    <row r="89" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>122</v>
       </c>
@@ -5165,7 +5162,7 @@
       </c>
       <c r="Q89" s="3"/>
     </row>
-    <row r="90" spans="1:18" ht="72" customHeight="1">
+    <row r="90" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>122</v>
       </c>
@@ -5215,7 +5212,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="91" spans="1:18" ht="72" customHeight="1">
+    <row r="91" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>122</v>
       </c>
@@ -5262,7 +5259,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="92" spans="1:18" ht="72" customHeight="1">
+    <row r="92" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>122</v>
       </c>
@@ -5309,7 +5306,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="93" spans="1:18" ht="72" customHeight="1">
+    <row r="93" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>122</v>
       </c>
@@ -5356,7 +5353,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="94" spans="1:18" ht="72" customHeight="1">
+    <row r="94" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>122</v>
       </c>
@@ -5403,7 +5400,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="95" spans="1:18" ht="72" customHeight="1">
+    <row r="95" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>122</v>
       </c>
@@ -5450,7 +5447,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="96" spans="1:18" ht="72" customHeight="1">
+    <row r="96" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>122</v>
       </c>
@@ -5497,7 +5494,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="97" spans="1:17" ht="72" customHeight="1">
+    <row r="97" spans="1:17" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>122</v>
       </c>
@@ -5544,7 +5541,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="98" spans="1:17" ht="72" customHeight="1">
+    <row r="98" spans="1:17" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>122</v>
       </c>
@@ -5591,7 +5588,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="99" spans="1:17" ht="72" customHeight="1">
+    <row r="99" spans="1:17" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>122</v>
       </c>
@@ -6043,21 +6040,21 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="27.4375" customWidth="1"/>
-    <col min="3" max="3" width="13.4375" customWidth="1"/>
-    <col min="4" max="4" width="10.875" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="46" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="42.5625" customWidth="1"/>
-    <col min="15" max="15" width="25.75" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="47.6875" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42.5703125" customWidth="1"/>
+    <col min="15" max="15" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="47.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="14.1" customHeight="1">
+    <row r="1" spans="1:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6110,10 +6107,10 @@
         <v>16</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" s="11" customFormat="1" ht="57.95" customHeight="1">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="11" customFormat="1" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>122</v>
       </c>
@@ -6130,7 +6127,7 @@
         <v>68</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>145</v>
@@ -6160,7 +6157,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="57.95" customHeight="1">
+    <row r="3" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>122</v>
       </c>
@@ -6177,7 +6174,7 @@
         <v>68</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>145</v>
@@ -6207,7 +6204,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="57.95" customHeight="1">
+    <row r="4" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>122</v>
       </c>
@@ -6224,7 +6221,7 @@
         <v>68</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>145</v>
@@ -6254,7 +6251,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="57.95" customHeight="1">
+    <row r="5" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>122</v>
       </c>
@@ -6271,7 +6268,7 @@
         <v>68</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>145</v>
@@ -6301,7 +6298,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="57.95" customHeight="1">
+    <row r="6" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>122</v>
       </c>
@@ -6318,7 +6315,7 @@
         <v>68</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>145</v>
@@ -6348,7 +6345,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="57.95" customHeight="1">
+    <row r="7" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>122</v>
       </c>
@@ -6365,7 +6362,7 @@
         <v>68</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>145</v>
@@ -6395,7 +6392,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="57.95" customHeight="1">
+    <row r="8" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>122</v>
       </c>
@@ -6412,7 +6409,7 @@
         <v>68</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>145</v>
@@ -6440,7 +6437,7 @@
       </c>
       <c r="Q8" s="3"/>
     </row>
-    <row r="9" spans="1:18" ht="57.95" customHeight="1">
+    <row r="9" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>122</v>
       </c>
@@ -6477,7 +6474,7 @@
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
     </row>
-    <row r="10" spans="1:18" ht="57.95" customHeight="1">
+    <row r="10" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>122</v>
       </c>
@@ -6522,7 +6519,7 @@
       </c>
       <c r="Q10" s="3"/>
     </row>
-    <row r="11" spans="1:18" ht="57.95" customHeight="1">
+    <row r="11" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>122</v>
       </c>
@@ -6567,7 +6564,7 @@
       </c>
       <c r="Q11" s="3"/>
     </row>
-    <row r="12" spans="1:18" ht="57.95" customHeight="1">
+    <row r="12" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>122</v>
       </c>
@@ -6614,7 +6611,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="57.95" customHeight="1">
+    <row r="13" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>122</v>
       </c>
@@ -6661,7 +6658,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="57.95" customHeight="1">
+    <row r="14" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>122</v>
       </c>
@@ -6706,7 +6703,7 @@
       </c>
       <c r="Q14" s="3"/>
     </row>
-    <row r="15" spans="1:18" ht="57.95" customHeight="1">
+    <row r="15" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>122</v>
       </c>
@@ -6751,7 +6748,7 @@
       </c>
       <c r="Q15" s="3"/>
     </row>
-    <row r="16" spans="1:18" ht="57.95" customHeight="1">
+    <row r="16" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>122</v>
       </c>
@@ -6798,7 +6795,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="57.95" customHeight="1">
+    <row r="17" spans="1:17" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>122</v>
       </c>
@@ -6845,7 +6842,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="57.95" customHeight="1">
+    <row r="18" spans="1:17" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>122</v>
       </c>
@@ -6890,7 +6887,7 @@
       </c>
       <c r="Q18" s="3"/>
     </row>
-    <row r="19" spans="1:17" ht="57.95" customHeight="1">
+    <row r="19" spans="1:17" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>122</v>
       </c>
@@ -6935,7 +6932,7 @@
       </c>
       <c r="Q19" s="3"/>
     </row>
-    <row r="20" spans="1:17" ht="57.95" customHeight="1">
+    <row r="20" spans="1:17" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>122</v>
       </c>
@@ -6982,7 +6979,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="57.95" customHeight="1">
+    <row r="21" spans="1:17" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>122</v>
       </c>
@@ -7029,7 +7026,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="57.95" customHeight="1">
+    <row r="22" spans="1:17" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>122</v>
       </c>
@@ -7074,7 +7071,7 @@
       </c>
       <c r="Q22" s="3"/>
     </row>
-    <row r="23" spans="1:17" ht="57.95" customHeight="1">
+    <row r="23" spans="1:17" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>122</v>
       </c>
@@ -7119,7 +7116,7 @@
       </c>
       <c r="Q23" s="3"/>
     </row>
-    <row r="24" spans="1:17" ht="57.95" customHeight="1">
+    <row r="24" spans="1:17" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>122</v>
       </c>
@@ -7166,7 +7163,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="57.95" customHeight="1">
+    <row r="25" spans="1:17" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>122</v>
       </c>
@@ -7213,18 +7210,18 @@
         <v>190</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="57.95" customHeight="1">
+    <row r="26" spans="1:17" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>122</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>177</v>
@@ -7233,13 +7230,13 @@
         <v>176</v>
       </c>
       <c r="G26" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="H26" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="H26" s="3" t="s">
-        <v>207</v>
-      </c>
       <c r="I26" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
@@ -7258,18 +7255,18 @@
       </c>
       <c r="Q26" s="3"/>
     </row>
-    <row r="27" spans="1:17" ht="57.95" customHeight="1">
+    <row r="27" spans="1:17" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>122</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>177</v>
@@ -7278,13 +7275,13 @@
         <v>176</v>
       </c>
       <c r="G27" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="H27" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="H27" s="3" t="s">
-        <v>207</v>
-      </c>
       <c r="I27" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
@@ -7303,18 +7300,18 @@
       </c>
       <c r="Q27" s="3"/>
     </row>
-    <row r="28" spans="1:17" ht="57.95" customHeight="1">
+    <row r="28" spans="1:17" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>122</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>177</v>
@@ -7323,13 +7320,13 @@
         <v>176</v>
       </c>
       <c r="G28" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="H28" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="H28" s="3" t="s">
-        <v>207</v>
-      </c>
       <c r="I28" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
@@ -7350,18 +7347,18 @@
         <v>182</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="57.95" customHeight="1">
+    <row r="29" spans="1:17" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>122</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>177</v>
@@ -7370,13 +7367,13 @@
         <v>176</v>
       </c>
       <c r="G29" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="H29" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="H29" s="3" t="s">
-        <v>207</v>
-      </c>
       <c r="I29" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
@@ -7394,7 +7391,7 @@
         <v>20</v>
       </c>
       <c r="Q29" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix Best Overall Response BC (C94536)
</commit_message>
<xml_diff>
--- a/curation/draft/BC_Package_R8_BC_updates.xlsx
+++ b/curation/draft/BC_Package_R8_BC_updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\curation\draft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC4852E-15EB-446F-A7BF-05E5C7923B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC2B80A-D54A-419C-ABB0-8BD4BEF5F8EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="390" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="390" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BC_Onco_Corrections" sheetId="2" r:id="rId1"/>
@@ -609,9 +609,6 @@
     <t>The determination of the amount of very low-density lipoprotein cholesterol present in a sample.</t>
   </si>
   <si>
-    <t>Oncology Standards; Disease Response; Disease Response Criteria; Disease Response and Clinical Classification; RS; RECIST 1.0; iRECIST</t>
-  </si>
-  <si>
     <t>Oncology Standards; Disease Response; Disease Response Criteria; Disease Response and Clinical Classification; RS; RECIST 1.1; iRECIST; RAJKUMAR MYELOMA 2011</t>
   </si>
   <si>
@@ -652,6 +649,9 @@
   </si>
   <si>
     <t>change_history</t>
+  </si>
+  <si>
+    <t>Oncology Standards; Disease Response; Disease Response Criteria; Disease Response and Clinical Classification; RS; RECIST 1.1; iRECIST</t>
   </si>
 </sst>
 </file>
@@ -951,7 +951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -1029,7 +1029,7 @@
         <v>16</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -1049,7 +1049,7 @@
         <v>23</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>24</v>
@@ -1099,7 +1099,7 @@
         <v>23</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>24</v>
@@ -1146,7 +1146,7 @@
         <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>24</v>
@@ -1193,7 +1193,7 @@
         <v>23</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>24</v>
@@ -1240,7 +1240,7 @@
         <v>23</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>24</v>
@@ -3058,7 +3058,7 @@
         <v>68</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>86</v>
@@ -3085,7 +3085,7 @@
         <v>20</v>
       </c>
       <c r="Q45" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="R45" t="s">
         <v>156</v>
@@ -3108,7 +3108,7 @@
         <v>68</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>86</v>
@@ -3155,7 +3155,7 @@
         <v>68</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>86</v>
@@ -3202,7 +3202,7 @@
         <v>68</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>86</v>
@@ -3249,7 +3249,7 @@
         <v>68</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>86</v>
@@ -3294,7 +3294,7 @@
         <v>68</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>90</v>
@@ -3321,7 +3321,7 @@
         <v>20</v>
       </c>
       <c r="Q50" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="R50" t="s">
         <v>156</v>
@@ -3344,7 +3344,7 @@
         <v>68</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>90</v>
@@ -3391,7 +3391,7 @@
         <v>68</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G52" s="3" t="s">
         <v>90</v>
@@ -3438,7 +3438,7 @@
         <v>68</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>90</v>
@@ -3485,7 +3485,7 @@
         <v>68</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>90</v>
@@ -3530,7 +3530,7 @@
         <v>68</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G55" s="3" t="s">
         <v>95</v>
@@ -3580,7 +3580,7 @@
         <v>68</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>95</v>
@@ -3607,7 +3607,7 @@
         <v>20</v>
       </c>
       <c r="Q56" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="57" spans="1:18" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -3627,7 +3627,7 @@
         <v>68</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>95</v>
@@ -3674,7 +3674,7 @@
         <v>68</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>95</v>
@@ -3721,7 +3721,7 @@
         <v>68</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G59" s="3" t="s">
         <v>95</v>
@@ -3768,7 +3768,7 @@
         <v>68</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G60" s="3" t="s">
         <v>95</v>
@@ -6036,8 +6036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCCE412A-0D79-4DD1-A165-132368A8F955}">
   <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6107,7 +6107,7 @@
         <v>16</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="11" customFormat="1" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -6127,7 +6127,7 @@
         <v>68</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>145</v>
@@ -6174,7 +6174,7 @@
         <v>68</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>145</v>
@@ -6221,7 +6221,7 @@
         <v>68</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>145</v>
@@ -6268,7 +6268,7 @@
         <v>68</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>145</v>
@@ -6315,7 +6315,7 @@
         <v>68</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>145</v>
@@ -6362,7 +6362,7 @@
         <v>68</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>145</v>
@@ -6409,7 +6409,7 @@
         <v>68</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>145</v>
@@ -7215,13 +7215,13 @@
         <v>122</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>177</v>
@@ -7230,13 +7230,13 @@
         <v>176</v>
       </c>
       <c r="G26" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="H26" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="H26" s="3" t="s">
-        <v>206</v>
-      </c>
       <c r="I26" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
@@ -7260,13 +7260,13 @@
         <v>122</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>177</v>
@@ -7275,13 +7275,13 @@
         <v>176</v>
       </c>
       <c r="G27" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="H27" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="H27" s="3" t="s">
-        <v>206</v>
-      </c>
       <c r="I27" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
@@ -7305,13 +7305,13 @@
         <v>122</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>177</v>
@@ -7320,13 +7320,13 @@
         <v>176</v>
       </c>
       <c r="G28" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="H28" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="H28" s="3" t="s">
-        <v>206</v>
-      </c>
       <c r="I28" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
@@ -7352,13 +7352,13 @@
         <v>122</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>177</v>
@@ -7367,13 +7367,13 @@
         <v>176</v>
       </c>
       <c r="G29" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="H29" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="H29" s="3" t="s">
-        <v>206</v>
-      </c>
       <c r="I29" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
@@ -7391,7 +7391,7 @@
         <v>20</v>
       </c>
       <c r="Q29" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>